<commit_message>
Extract data from all pdf of the folder 18-09-2023
</commit_message>
<xml_diff>
--- a/OutPut.xlsx
+++ b/OutPut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadha\Documents\UiPath\Document_underStanding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608EB7EC-01AF-480E-82B8-69E23E098DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAE4384-6948-425E-87CC-857DAA768C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
+  <si>
+    <t>Invoice_Number</t>
+  </si>
+  <si>
+    <t>Invoice_date</t>
+  </si>
+  <si>
+    <t>GSTN</t>
+  </si>
   <si>
     <t>Invoice_number</t>
   </si>
@@ -33,7 +42,13 @@
     <t>Invoice_Date</t>
   </si>
   <si>
-    <t>GSTN</t>
+    <t>INM01396/2023-24</t>
+  </si>
+  <si>
+    <t>2023-06-02</t>
+  </si>
+  <si>
+    <t>24AABCL5045N1ZE</t>
   </si>
   <si>
     <t>HDF232452W/R001</t>
@@ -43,6 +58,138 @@
   </si>
   <si>
     <t>27AABCL5045N1Z8</t>
+  </si>
+  <si>
+    <t>HDFCOO12O23</t>
+  </si>
+  <si>
+    <t>2023-08-09</t>
+  </si>
+  <si>
+    <t>36AABCL5045N1Z9</t>
+  </si>
+  <si>
+    <t>AR/MH/G2324/0016</t>
+  </si>
+  <si>
+    <t>2023-04-07</t>
+  </si>
+  <si>
+    <t>BIBPL/D23-24/61</t>
+  </si>
+  <si>
+    <t>2023-06-16</t>
+  </si>
+  <si>
+    <t>CYP/23-24/0022</t>
+  </si>
+  <si>
+    <t>2023-07-11</t>
+  </si>
+  <si>
+    <t>2902</t>
+  </si>
+  <si>
+    <t>G/HO/23-24/00059</t>
+  </si>
+  <si>
+    <t>2023-08-10</t>
+  </si>
+  <si>
+    <t>2324/36/0000096</t>
+  </si>
+  <si>
+    <t>2023-06-12</t>
+  </si>
+  <si>
+    <t>GIC/HDFC/AUG/04</t>
+  </si>
+  <si>
+    <t>MH/0923TWBU/0006</t>
+  </si>
+  <si>
+    <t>2023-09-02</t>
+  </si>
+  <si>
+    <t>NO-2023-24/GN/88</t>
+  </si>
+  <si>
+    <t>NO-27AABCL5045N1Z8</t>
+  </si>
+  <si>
+    <t>MIC-Jun-23-001</t>
+  </si>
+  <si>
+    <t>PIPKAI2400000086</t>
+  </si>
+  <si>
+    <t>2023-07-26</t>
+  </si>
+  <si>
+    <t>29AABCL5045N1Z4</t>
+  </si>
+  <si>
+    <t>FY-23-24-PX-099</t>
+  </si>
+  <si>
+    <t>2023-08-24</t>
+  </si>
+  <si>
+    <t>1232401057</t>
+  </si>
+  <si>
+    <t>2023-07-06</t>
+  </si>
+  <si>
+    <t>G/HO/2324/00123</t>
+  </si>
+  <si>
+    <t>2023-08-28</t>
+  </si>
+  <si>
+    <t>06AABCL5045N1ZC</t>
+  </si>
+  <si>
+    <t>SIBPL/00034</t>
+  </si>
+  <si>
+    <t>2023-07-14</t>
+  </si>
+  <si>
+    <t>99102</t>
+  </si>
+  <si>
+    <t>2020-08-15</t>
+  </si>
+  <si>
+    <t>2023/Jul/2</t>
+  </si>
+  <si>
+    <t>2023-07-27</t>
+  </si>
+  <si>
+    <t>INV23-24/2621</t>
+  </si>
+  <si>
+    <t>9859</t>
+  </si>
+  <si>
+    <t>2023-08-13</t>
+  </si>
+  <si>
+    <t>VIBPL/23-24/0182</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>23-24/YL/181</t>
+  </si>
+  <si>
+    <t>2023-07-13</t>
+  </si>
+  <si>
+    <t>32AABCL5045N1ZH</t>
   </si>
 </sst>
 </file>
@@ -360,20 +507,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,16 +532,410 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>